<commit_message>
will decide the times later
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F90968F4-848F-4553-AB12-E898D4A06B7A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B1924976-A794-4D23-8D89-EBD835FE1EE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Tasks</t>
   </si>
@@ -91,15 +91,6 @@
   </si>
   <si>
     <t>End date</t>
-  </si>
-  <si>
-    <t>till Oct 7</t>
-  </si>
-  <si>
-    <t>till Oct 10</t>
-  </si>
-  <si>
-    <t>till Oct 14</t>
   </si>
 </sst>
 </file>
@@ -472,7 +463,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,9 +510,6 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -536,9 +524,6 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -553,9 +538,6 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -569,9 +551,6 @@
       </c>
       <c r="D5">
         <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updating tasks and people working
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B1924976-A794-4D23-8D89-EBD835FE1EE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F0CD107-976B-4ED1-9B48-E01766A4F7F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Tasks</t>
   </si>
@@ -90,14 +90,38 @@
     <t>Research</t>
   </si>
   <si>
-    <t>End date</t>
+    <t>Devershi</t>
+  </si>
+  <si>
+    <t>Yelp business json processing</t>
+  </si>
+  <si>
+    <t>Rimsha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crawling to get inspection/voilations </t>
+  </si>
+  <si>
+    <t>Rajdeep/Ajay</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>Working</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +133,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -146,6 +177,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,11 +508,12 @@
     <col min="2" max="2" width="62.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -492,26 +529,28 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -524,8 +563,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -538,83 +583,101 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -623,12 +686,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -637,17 +700,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding completion date in tasks
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F0CD107-976B-4ED1-9B48-E01766A4F7F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7DC9B1EF-2099-4DC6-ACD8-6E98D95E0B89}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Tasks</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Working</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -182,6 +185,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,10 +514,10 @@
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -532,8 +536,11 @@
       <c r="F1" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -549,8 +556,11 @@
       <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="8">
+        <v>43379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -570,7 +580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -590,7 +600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -607,7 +617,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -624,7 +634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -640,8 +650,11 @@
       <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G7" s="8">
+        <v>43379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -658,7 +671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -672,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -686,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -700,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -714,7 +727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -728,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Updated code for las Vegas Data
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{90B8A4CF-DF55-484F-A652-717E1CAEE44D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{425B7586-000E-4619-BCAE-A5DF2F8D82BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Tasks</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Data exploration</t>
   </si>
   <si>
-    <t>Isolate LA data from yelp data - coding</t>
-  </si>
-  <si>
     <t>Data collection</t>
   </si>
   <si>
@@ -136,6 +133,24 @@
   </si>
   <si>
     <t>Data mining</t>
+  </si>
+  <si>
+    <t>Find missing columns for each business_id. Eg business_id : 3,[column1, column2, column3]</t>
+  </si>
+  <si>
+    <t>Isolate data according to states and Las Vegas from yelp data - coding</t>
+  </si>
+  <si>
+    <t>Rajdeep</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Rajdeep and Rimsha</t>
+  </si>
+  <si>
+    <t>Devershi!!!???</t>
   </si>
 </sst>
 </file>
@@ -521,24 +536,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="62.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -555,13 +570,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -575,33 +590,33 @@
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="8">
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,56 +624,59 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -666,19 +684,22 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="F7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="8">
         <v>43379</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -686,16 +707,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -703,50 +724,56 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -754,8 +781,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -768,8 +798,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -782,8 +815,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -796,8 +832,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -810,19 +849,25 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
       <c r="D17">
         <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving data under resources
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553-YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{425B7586-000E-4619-BCAE-A5DF2F8D82BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{39D3C17B-00EB-49BA-8089-5177FE2AE911}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Tasks</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Code to find data overlap - yelp and govt data, and creating final dataset for us</t>
   </si>
   <si>
-    <t>For LA yelp data, Find how much missing data exist - which restaurants have all data missing, some data missing - separate missing data vs clean data</t>
-  </si>
-  <si>
     <t>Data analysis</t>
   </si>
   <si>
@@ -144,13 +141,13 @@
     <t>Rajdeep</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Rajdeep and Rimsha</t>
   </si>
   <si>
     <t>Devershi!!!???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Las Vegas yelp data, Find how much missing data exist - which restaurants have all data missing, some data missing </t>
   </si>
 </sst>
 </file>
@@ -538,22 +535,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -561,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>6</v>
@@ -570,13 +567,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -584,99 +581,99 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="8">
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -684,22 +681,19 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="8">
         <v>43379</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -707,16 +701,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -724,150 +718,150 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated task list with new tasks for data analysis and ML
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{39D3C17B-00EB-49BA-8089-5177FE2AE911}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{443F76A9-F11C-4079-A549-02115B68DDDE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="October" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Tasks</t>
   </si>
@@ -60,15 +60,6 @@
     <t>Type of task</t>
   </si>
   <si>
-    <t>Find statistics of Grade vs number of restaurants</t>
-  </si>
-  <si>
-    <t>Find statistics of health score vs number of restaurants</t>
-  </si>
-  <si>
-    <t>Find statistics of region vs number of restaurants</t>
-  </si>
-  <si>
     <t>Data exploration</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t xml:space="preserve">Crawling to get inspection/voilations </t>
   </si>
   <si>
-    <t>Rajdeep/Ajay</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -126,9 +114,6 @@
     <t>Find feature importance (using Pearson coefficient or other) and check which features are more useful - may require reading literature</t>
   </si>
   <si>
-    <t>Find best metric to determine similarity between features and coding</t>
-  </si>
-  <si>
     <t>Data mining</t>
   </si>
   <si>
@@ -148,6 +133,45 @@
   </si>
   <si>
     <t xml:space="preserve">For Las Vegas yelp data, Find how much missing data exist - which restaurants have all data missing, some data missing </t>
+  </si>
+  <si>
+    <t>Postponed this task. Not required for now</t>
+  </si>
+  <si>
+    <t>Find best metric for similarity matching and Python script for similarity matching among final features</t>
+  </si>
+  <si>
+    <t>Rajdeep and Ajay</t>
+  </si>
+  <si>
+    <t>Python script to find statistics of region vs number of restaurants</t>
+  </si>
+  <si>
+    <t>Python script to find mean score of restaurant for each zip code - Useful to show which regions perform good and which perform bad generally</t>
+  </si>
+  <si>
+    <t>Python script to plot graph between feature values (x-axis) vs health score (y-axis) - for each feature to be used in training - For e.g It is useful to determine what is the mean score of restaurant with rating 1, what is mean score of restaurant with rating 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Python script to find statistics and plot graph of Grade vs number of restaurants - Useful to find how many restaurant have grade A, how many have B, C, D, …</t>
+  </si>
+  <si>
+    <t>Python script to find statistics and plot graph of health score vs number of restaurants - Useful to find how many restaurants have Health Score between 90-100, how many have score between 80-90, …</t>
+  </si>
+  <si>
+    <t>Python script to divide dataset into training, validation, and test set</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Python script to save and load the model - Useful for future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python script to plot ROC and AUC </t>
+  </si>
+  <si>
+    <t>Python script to determine TP, TN, FP, FN, Sensitivity (recall), Specificity, precision, F1 score, Accuracy</t>
   </si>
 </sst>
 </file>
@@ -198,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,6 +241,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +575,7 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="62.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="9" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -567,10 +598,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -581,13 +612,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5">
+        <v>11</v>
+      </c>
+      <c r="D2" s="12">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8">
         <v>43379</v>
@@ -598,19 +629,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -618,22 +649,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -641,19 +672,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -661,16 +692,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="G6" s="11">
+        <v>43384</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -681,13 +712,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5">
+        <v>12</v>
+      </c>
+      <c r="D7" s="12">
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8">
         <v>43379</v>
@@ -701,13 +732,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -718,16 +746,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -735,16 +763,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="9">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -752,14 +783,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="D11" s="10"/>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -767,16 +798,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -789,79 +820,166 @@
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>11</v>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="9">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="8">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added region wise counts csv
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C6B2E5BC-4902-43A1-BCAB-1A38121C6C39}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{685B765F-4EEA-4DBB-B18F-3F0DFF073594}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>Tasks</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Python script for model based/ user based matching and fill data</t>
+  </si>
+  <si>
+    <t>Added state wise count</t>
   </si>
 </sst>
 </file>
@@ -576,21 +579,21 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="62.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -613,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -633,7 +636,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -653,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -676,7 +679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -696,7 +699,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -714,7 +717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -731,7 +734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -751,7 +754,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -765,7 +768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -785,7 +788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -805,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -820,7 +823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -837,7 +840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -854,7 +857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -871,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -888,7 +891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -904,11 +907,17 @@
       <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="8">
         <v>43384</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -925,7 +934,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -939,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -953,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -967,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -981,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1009,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
APIs created to retrieve ML evaluation metrics based on actual vs predicted data
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B87DF222-0C6C-40F6-BB4A-C03F6424EDA3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A79E9E7-8BF9-4648-82ED-CAD533359CCD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04F21BEB-744F-48B2-975A-B4915A3A764F}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -150,15 +150,9 @@
     <t>Python script to find statistics and plot graph of health score vs number of restaurants - Useful to find how many restaurants have Health Score between 90-100, how many have score between 80-90, …</t>
   </si>
   <si>
-    <t>Python script to divide dataset into training, validation, and test set</t>
-  </si>
-  <si>
     <t>Machine Learning</t>
   </si>
   <si>
-    <t>Python script to save and load the model - Useful for future</t>
-  </si>
-  <si>
     <t xml:space="preserve">Python script to plot ROC and AUC </t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>(~\(' v ')/~)</t>
+  </si>
+  <si>
+    <t>Python script to save and load the model - Total 2 APIs</t>
+  </si>
+  <si>
+    <t>Python script to divide dataset into training, validation, and test set - One API</t>
   </si>
 </sst>
 </file>
@@ -595,22 +595,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F0EF69-C05F-4321-87D8-BBE5325B227C}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -633,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -653,7 +653,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -673,12 +673,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -690,18 +690,18 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -713,13 +713,13 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -739,12 +739,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -757,7 +757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -774,7 +774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -794,7 +794,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -808,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -828,7 +828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -848,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -863,7 +863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -880,7 +880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -897,10 +897,10 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -917,7 +917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -934,7 +934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -957,15 +957,15 @@
         <v>43384</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -977,15 +977,15 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -994,10 +994,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1031,15 +1031,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="8">
         <v>1</v>
@@ -1048,15 +1048,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
@@ -1065,15 +1065,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="8">
         <v>1</v>
@@ -1082,15 +1082,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>

</xml_diff>

<commit_message>
Minor changes to code
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F9A8F1A-42D3-4DDD-8366-7BDB862A672D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D2C707A1-EB8F-4A8F-B05B-6D2062E78154}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="72">
   <si>
     <t>S.No</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>save evaluation metric for each restaurant</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
   </si>
 </sst>
 </file>
@@ -290,9 +293,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,6 +317,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +637,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,76 +645,76 @@
     <col min="1" max="1" width="5"/>
     <col min="2" max="2" width="63.140625"/>
     <col min="3" max="3" width="16.85546875"/>
-    <col min="4" max="4" width="12.85546875" style="2"/>
+    <col min="4" max="4" width="12.85546875" style="1"/>
     <col min="5" max="5" width="18.85546875"/>
     <col min="6" max="6" width="8.7109375"/>
     <col min="7" max="7" width="15.5703125"/>
     <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>43379</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>43392</v>
       </c>
     </row>
@@ -719,13 +722,13 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
+        <v>71</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" t="s">
@@ -739,52 +742,52 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
@@ -802,45 +805,45 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>43384</v>
       </c>
       <c r="H8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>43379</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
@@ -855,13 +858,13 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -875,13 +878,13 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="13">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -895,28 +898,28 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="13"/>
       <c r="E13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -927,13 +930,13 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" t="s">
@@ -947,62 +950,62 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>43384</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1010,13 +1013,13 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" t="s">
@@ -1030,13 +1033,13 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" t="s">
@@ -1047,13 +1050,13 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" t="s">
@@ -1061,16 +1064,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" t="s">
@@ -1081,13 +1084,13 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -1098,71 +1101,71 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="7">
-        <v>1</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="8"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="H27" t="s">
@@ -1170,16 +1173,16 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="H28" t="s">
@@ -1187,16 +1190,16 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C29" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="H29" t="s">
@@ -1204,16 +1207,16 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="H30" t="s">
@@ -1221,16 +1224,16 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="H31" t="s">
@@ -1238,16 +1241,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C32" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="H32" t="s">
@@ -1255,7 +1258,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="11"/>
       <c r="H33" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
added detailed analysis for missing data(full, partial)
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D2C707A1-EB8F-4A8F-B05B-6D2062E78154}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8E2DA146-CA75-4A3C-AAD2-84AFC5BE7873}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>S.No</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve">For Las Vegas yelp data, Find how much missing data exist - which restaurants have all data missing, some data missing  </t>
-  </si>
-  <si>
-    <t>Priority1</t>
   </si>
   <si>
     <t>Find missing columns for each business_id. Eg business_id : 3,[column1, column2, column3]</t>
@@ -634,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +649,7 @@
     <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -675,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -695,7 +692,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -718,35 +715,45 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -762,12 +769,12 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -776,58 +783,58 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10">
         <v>43384</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
@@ -839,27 +846,27 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -868,73 +875,73 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
       <c r="D12" s="13">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -943,24 +950,24 @@
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -968,16 +975,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>9</v>
@@ -988,10 +995,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -1006,7 +1013,7 @@
         <v>43384</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1014,10 +1021,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
         <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1026,7 +1033,7 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1034,16 +1041,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1051,10 +1058,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1068,16 +1075,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1085,16 +1092,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1102,16 +1109,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1119,16 +1126,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>9</v>
@@ -1140,10 +1147,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1152,7 +1159,7 @@
         <v>12</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1160,16 +1167,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1177,16 +1184,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
         <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,16 +1201,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,16 +1218,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,16 +1235,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,22 +1252,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
         <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="H33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated task list with expected deadline
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{306C0DDE-3CA0-4D28-88A2-829791FADAA5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{85CBCBB5-785B-451F-9A1F-B2182013913D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
+    <sheet name="November" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="75">
   <si>
     <t>S.No</t>
   </si>
@@ -238,6 +239,18 @@
   </si>
   <si>
     <t>save evaluation metric for each restaurant</t>
+  </si>
+  <si>
+    <t>Planned deadline</t>
+  </si>
+  <si>
+    <t>Devershi and Rajdeep</t>
+  </si>
+  <si>
+    <t>Get LA county dataset and prepare all data</t>
+  </si>
+  <si>
+    <t>Ajay and Rimsha</t>
   </si>
 </sst>
 </file>
@@ -247,7 +260,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -277,6 +290,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,6 +352,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,23 +746,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="A23:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.85546875"/>
+    <col min="2" max="2" width="58.88671875"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.7109375"/>
-    <col min="7" max="7" width="15.5703125"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="6" max="6" width="8.6640625"/>
+    <col min="7" max="7" width="15.5546875"/>
+    <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -756,7 +785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -776,7 +805,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -799,7 +828,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -834,7 +863,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -857,7 +886,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -880,7 +909,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -898,7 +927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -922,7 +951,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -942,7 +971,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -957,7 +986,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -977,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -997,7 +1026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1011,8 +1040,11 @@
       <c r="E13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1029,7 +1061,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1046,7 +1078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1066,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1092,7 +1124,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1115,7 +1147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1132,7 +1164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1157,7 +1189,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1173,8 +1205,11 @@
       <c r="E21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1191,7 +1226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1214,7 +1249,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1237,7 +1272,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1263,7 +1298,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1283,7 +1318,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1299,11 +1334,14 @@
       <c r="E27" t="s">
         <v>31</v>
       </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
       <c r="H27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1323,7 +1361,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1349,7 +1387,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1369,7 +1407,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1386,17 +1424,589 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D12:D13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E969FF-CFB6-45E6-832C-0B9279DA572C}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>6</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="25">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>7</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22">
+        <v>43384</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="19" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="25">
+        <v>43405</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24">
+        <v>11</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="25">
+        <v>43412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>12</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="25">
+        <v>43412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="25">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>14</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="25">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="24">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="25">
+        <v>43405</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24">
+        <v>17</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="25">
+        <v>43412</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24">
+        <v>18</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="25">
+        <v>43412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="24">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="25">
+        <v>43405</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="24">
+        <v>20</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="25">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24">
+        <v>21</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="25">
+        <v>43412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>22</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="25">
+        <v>43412</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>24</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="25">
+        <v>43412</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24">
+        <v>25</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="25">
+        <v>43416</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24">
+        <v>26</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="25">
+        <v>43416</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24">
+        <v>27</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="25">
+        <v>43416</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24">
+        <v>28</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="25">
+        <v>43416</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24">
+        <v>29</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="25">
+        <v>43419</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>30</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="25">
+        <v>43419</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="24">
+        <v>31</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="25">
+        <v>43416</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating assignee for task 31
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{85CBCBB5-785B-451F-9A1F-B2182013913D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{09FC29EE-0486-4D9D-B4E1-96A65AAE06D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
     <t>Get LA county dataset and prepare all data</t>
   </si>
   <si>
-    <t>Ajay and Rimsha</t>
+    <t>Ajay, will need Rimsha's help</t>
   </si>
 </sst>
 </file>
@@ -352,9 +352,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -362,6 +359,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E969FF-CFB6-45E6-832C-0B9279DA572C}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,7 +1450,7 @@
     <col min="2" max="2" width="64.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" customWidth="1"/>
   </cols>
@@ -1482,63 +1482,63 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="24">
         <v>43405</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
+    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
         <v>7</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21">
         <v>43384</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="19" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24">
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24">
+    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1556,98 +1556,98 @@
       <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <v>43405</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24">
+    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
         <v>11</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="18">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24">
+    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
         <v>12</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+    <row r="8" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
         <v>13</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <v>43405</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24">
+    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
         <v>14</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <v>43405</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="24">
+    <row r="10" spans="1:9" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1665,60 +1665,60 @@
       <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <v>43405</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24">
+    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
         <v>17</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="24">
         <v>43412</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24">
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
         <v>18</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="24">
         <v>43412</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1736,7 +1736,7 @@
       <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="24">
         <v>43405</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -1744,50 +1744,50 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="24">
+    <row r="14" spans="1:9" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
         <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="24">
         <v>43405</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
+    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
         <v>21</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="24">
         <v>43412</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1806,179 +1806,179 @@
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="24">
         <v>43412</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="24">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
         <v>24</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="24">
         <v>43412</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
         <v>25</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="24">
         <v>43416</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
         <v>26</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="24">
         <v>43416</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23">
         <v>27</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="24">
         <v>43416</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23">
         <v>28</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="24">
         <v>43416</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23">
         <v>29</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="24">
         <v>43419</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="A23" s="18">
         <v>30</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="25">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="24">
         <v>43419</v>
       </c>
       <c r="I23" t="s">
@@ -1986,20 +1986,20 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <v>31</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="24">
         <v>43416</v>
       </c>
     </row>

</xml_diff>

<commit_message>
API to split data for training, test, validation
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2868E915-A028-4F52-B69A-D37843BD0405}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" tabRatio="990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>S.No</t>
   </si>
@@ -265,7 +264,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -374,10 +373,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,26 +758,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G23" sqref="A23:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.88671875"/>
+    <col min="2" max="2" width="58.89453125"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.6640625"/>
-    <col min="7" max="7" width="15.5546875"/>
-    <col min="8" max="1025" width="8.5546875"/>
+    <col min="6" max="6" width="8.68359375"/>
+    <col min="7" max="7" width="15.5234375"/>
+    <col min="8" max="1025" width="8.5234375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -801,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -821,7 +820,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -844,7 +843,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -879,7 +878,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -902,7 +901,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -925,7 +924,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -943,7 +942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
@@ -967,7 +966,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -987,7 +986,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1042,7 +1041,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1114,7 +1113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1205,7 +1204,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1225,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1288,7 +1287,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1423,7 +1422,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
@@ -1453,25 +1452,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E969FF-CFB6-45E6-832C-0B9279DA572C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="64.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.3125" customWidth="1"/>
+    <col min="2" max="2" width="64.89453125" customWidth="1"/>
+    <col min="3" max="3" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5234375" customWidth="1"/>
+    <col min="5" max="5" width="24.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.68359375" customWidth="1"/>
+    <col min="8" max="8" width="12.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1498,7 +1497,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="18">
         <v>6</v>
       </c>
@@ -1522,7 +1521,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="23">
         <v>9</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="23">
         <v>10</v>
       </c>
@@ -1584,7 +1583,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="23">
         <v>11</v>
       </c>
@@ -1594,7 +1593,7 @@
       <c r="C6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="28">
         <v>1</v>
       </c>
       <c r="E6" s="18" t="s">
@@ -1607,7 +1606,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="23">
         <v>12</v>
       </c>
@@ -1617,7 +1616,7 @@
       <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="18" t="s">
         <v>31</v>
       </c>
@@ -1628,7 +1627,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="23">
         <v>13</v>
       </c>
@@ -1644,11 +1643,14 @@
       <c r="E8" s="18" t="s">
         <v>37</v>
       </c>
+      <c r="F8" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="24">
         <v>43405</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="23">
         <v>14</v>
       </c>
@@ -1668,7 +1670,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="23">
         <v>15</v>
       </c>
@@ -1695,7 +1697,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="23">
         <v>17</v>
       </c>
@@ -1724,7 +1726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="23">
         <v>18</v>
       </c>
@@ -1744,7 +1746,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="23">
         <v>19</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1789,34 +1791,40 @@
       <c r="F14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="27">
         <v>43405</v>
       </c>
       <c r="H14" s="24">
         <v>43407</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6">
         <v>21</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="24">
+      <c r="F15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="27">
         <v>43412</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="27">
+        <v>43410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1835,17 +1843,17 @@
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="27">
         <v>43412</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <v>43407</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="23">
         <v>24</v>
       </c>
@@ -1871,7 +1879,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="23">
         <v>25</v>
       </c>
@@ -1894,7 +1902,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="23">
         <v>26</v>
       </c>
@@ -1920,7 +1928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="23">
         <v>27</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="23">
         <v>28</v>
       </c>
@@ -1972,7 +1980,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="23">
         <v>29</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="18">
         <v>30</v>
       </c>
@@ -2014,7 +2022,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="23">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
updating status to completed for task 11
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{243510AD-8DDE-4EB4-AE20-8504BF14D4EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -264,7 +265,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
@@ -758,26 +759,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G23" sqref="A23:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.89453125"/>
+    <col min="2" max="2" width="58.88671875"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.68359375"/>
-    <col min="7" max="7" width="15.5234375"/>
-    <col min="8" max="1025" width="8.5234375"/>
+    <col min="6" max="6" width="8.6640625"/>
+    <col min="7" max="7" width="15.5546875"/>
+    <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -800,7 +801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -820,7 +821,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -843,7 +844,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -878,7 +879,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -901,7 +902,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -924,7 +925,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -942,7 +943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -966,7 +967,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -986,7 +987,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1204,7 +1205,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1376,7 +1377,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
@@ -1452,25 +1453,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.3125" customWidth="1"/>
-    <col min="2" max="2" width="64.89453125" customWidth="1"/>
-    <col min="3" max="3" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5234375" customWidth="1"/>
-    <col min="5" max="5" width="24.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.68359375" customWidth="1"/>
-    <col min="8" max="8" width="12.68359375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1498,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>6</v>
       </c>
@@ -1521,7 +1522,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>9</v>
       </c>
@@ -1556,7 +1557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>10</v>
       </c>
@@ -1583,30 +1584,30 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="23">
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>11</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="28">
         <v>1</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="24">
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="27">
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>12</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>13</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>14</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" s="18" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>15</v>
       </c>
@@ -1697,7 +1698,7 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>17</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>18</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>19</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>21</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>24</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>25</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>26</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>27</v>
       </c>
@@ -1954,7 +1955,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>28</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>29</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>30</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Updating status of task 12 to completed
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{243510AD-8DDE-4EB4-AE20-8504BF14D4EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C6869568-7559-4977-8FAC-756C03830766}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1607,24 +1607,24 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23">
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>12</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="28"/>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="24">
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="27">
         <v>43412</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scripts for graph plots
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3FB58234-82CF-4110-B819-91722A27CAEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F5868644-C08F-45E7-8726-14F41D001A09}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1447,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Postal Code wise Analysis data files
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{41D9AF36-BD60-437B-8E54-DABB6608F805}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F01E3D58-4D87-4BB2-83C6-B08DB3103159}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updating task list with completed tasks
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F01E3D58-4D87-4BB2-83C6-B08DB3103159}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80602FD4-07CA-4463-8DFC-F0B529132C8C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6828" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="81">
   <si>
     <t>S.No</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>ALS -&gt; Datamining assignment</t>
+  </si>
+  <si>
+    <t>Merge scraped data from Yelp with final dataset - add new useful features found after scraping + fill missing data using scraping</t>
+  </si>
+  <si>
+    <t>Done by Ajay</t>
   </si>
 </sst>
 </file>
@@ -372,7 +378,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -760,22 +766,22 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="A23:G23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.85546875"/>
+    <col min="2" max="2" width="58.88671875"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.7109375"/>
-    <col min="7" max="7" width="15.5703125"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="6" max="6" width="8.6640625"/>
+    <col min="7" max="7" width="15.5546875"/>
+    <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -798,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -818,7 +824,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -841,7 +847,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -876,7 +882,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -899,7 +905,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -922,7 +928,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -940,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -964,7 +970,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -984,7 +990,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1202,7 +1208,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1331,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1400,7 +1406,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
@@ -1453,22 +1459,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1495,8 +1501,8 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1505,21 +1511,20 @@
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="25">
         <v>43405</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="25">
         <v>43407</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -1540,22 +1545,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="18" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
-        <v>9</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="I4" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1573,15 +1581,14 @@
       <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="25">
         <v>43405</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="25">
         <v>43407</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>11</v>
       </c>
@@ -1604,12 +1611,12 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>34</v>
+      <c r="B7" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
@@ -1625,7 +1632,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>13</v>
       </c>
@@ -1648,7 +1655,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>14</v>
       </c>
@@ -1668,8 +1675,8 @@
         <v>43781</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1687,15 +1694,14 @@
       <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="25">
         <v>43405</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="25">
         <v>43407</v>
       </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>17</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>18</v>
       </c>
@@ -1747,7 +1753,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>19</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1796,11 +1802,11 @@
       <c r="G14" s="25">
         <v>43405</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="25">
         <v>43407</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>21</v>
       </c>
@@ -1826,7 +1832,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1855,7 +1861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>24</v>
       </c>
@@ -1881,7 +1887,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>25</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>26</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>27</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>28</v>
       </c>
@@ -1982,7 +1988,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>29</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>30</v>
       </c>
@@ -2024,7 +2030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
adding completion status of tasks
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80602FD4-07CA-4463-8DFC-F0B529132C8C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7CF75B8-D9B1-41B0-8E0D-C16532D0AF10}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6828" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="81">
   <si>
     <t>S.No</t>
   </si>
@@ -766,7 +766,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,6 +1558,9 @@
       <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="I4" s="6" t="s">
         <v>80</v>
       </c>
@@ -1610,6 +1613,9 @@
       <c r="G6" s="25">
         <v>43412</v>
       </c>
+      <c r="H6" s="25">
+        <v>43412</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
@@ -1631,6 +1637,9 @@
       <c r="G7" s="25">
         <v>43412</v>
       </c>
+      <c r="H7" s="25">
+        <v>43412</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
@@ -1654,6 +1663,9 @@
       <c r="G8" s="25">
         <v>43405</v>
       </c>
+      <c r="H8" s="25">
+        <v>43412</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
@@ -1674,6 +1686,9 @@
       <c r="G9" s="24">
         <v>43781</v>
       </c>
+      <c r="H9" s="18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
@@ -1775,7 +1790,9 @@
       <c r="G13" s="25">
         <v>43412</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="25">
+        <v>43412</v>
+      </c>
       <c r="I13" s="6" t="s">
         <v>75</v>
       </c>
@@ -1883,6 +1900,9 @@
       <c r="G17" s="24">
         <v>43412</v>
       </c>
+      <c r="H17" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="18" t="s">
         <v>58</v>
       </c>
@@ -1931,6 +1951,9 @@
       </c>
       <c r="G19" s="24">
         <v>43416</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
update task list and use sklearn confusion matrix
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCE32FE8-FE28-493F-8FFB-4801C6EF97B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{99434065-607B-47A8-B9AC-FEAAEE9011F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6828" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="87">
   <si>
     <t>S.No</t>
   </si>
@@ -269,6 +269,24 @@
   </si>
   <si>
     <t>ALS -&gt; Datamining assignment, Try out the pearson and cosine similarity metrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT cleaning - remove unnecessary files, make proper folder structures, insight section, etc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo workflow - end-to-end demo of project - make code changes or test app or ui app or set of APIs </t>
+  </si>
+  <si>
+    <t>Report - collect all stats, data analysis results, graphs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report preparation and writing </t>
+  </si>
+  <si>
+    <t>Presentation preparation - ppt/verbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual contributions - 5-10 points to be written by everyone and send to Rimsha </t>
   </si>
 </sst>
 </file>
@@ -769,19 +787,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.85546875"/>
+    <col min="2" max="2" width="58.88671875"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.7109375"/>
-    <col min="7" max="7" width="15.5703125"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="6" max="6" width="8.6640625"/>
+    <col min="7" max="7" width="15.5546875"/>
+    <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -804,7 +822,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -824,7 +842,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -847,7 +865,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -882,7 +900,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -905,7 +923,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -928,7 +946,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -946,7 +964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -970,7 +988,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -990,7 +1008,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1005,7 +1023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1025,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1080,7 +1098,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1097,7 +1115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1117,7 +1135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1143,7 +1161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1166,7 +1184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1183,7 +1201,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1208,7 +1226,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1245,7 +1263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1268,7 +1286,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1291,7 +1309,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1317,7 +1335,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1337,7 +1355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1360,7 +1378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1380,7 +1398,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1406,7 +1424,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1426,7 +1444,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
@@ -1457,24 +1475,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1501,7 +1519,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>6</v>
       </c>
@@ -1524,7 +1542,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -1545,7 +1563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>9</v>
       </c>
@@ -1565,7 +1583,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>10</v>
       </c>
@@ -1591,7 +1609,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>11</v>
       </c>
@@ -1617,7 +1635,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>12</v>
       </c>
@@ -1641,7 +1659,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>13</v>
       </c>
@@ -1667,7 +1685,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>14</v>
       </c>
@@ -1690,7 +1708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>15</v>
       </c>
@@ -1716,7 +1734,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>17</v>
       </c>
@@ -1748,7 +1766,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>18</v>
       </c>
@@ -1771,7 +1789,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>19</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1826,7 +1844,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>21</v>
       </c>
@@ -1852,7 +1870,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1881,7 +1899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>24</v>
       </c>
@@ -1910,7 +1928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>25</v>
       </c>
@@ -1933,7 +1951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>26</v>
       </c>
@@ -1962,7 +1980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>27</v>
       </c>
@@ -1988,7 +2006,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>28</v>
       </c>
@@ -2014,7 +2032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>29</v>
       </c>
@@ -2034,7 +2052,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>30</v>
       </c>
@@ -2056,7 +2074,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>31</v>
       </c>
@@ -2072,6 +2090,39 @@
       </c>
       <c r="G24" s="24">
         <v>43416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated assignee for new tasks
</commit_message>
<xml_diff>
--- a/Overview_and_Updates/Task Management.xlsx
+++ b/Overview_and_Updates/Task Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education_and_Work\Masters\Fall 2018\Foundations of Data Mining\Project\INF553_YelpProject\Overview_and_Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USC\courses\Fall_2018\Data_mining\project\yelp_git\INF553-YelpProject\Overview_and_Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E71F2EC0-7046-4806-8763-D456882F166F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B6A6C4D-FB62-42B7-B3E8-2DA2B2CE4CD3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6828" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="88">
   <si>
     <t>S.No</t>
   </si>
@@ -790,19 +790,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5"/>
-    <col min="2" max="2" width="58.85546875"/>
+    <col min="2" max="2" width="58.88671875"/>
     <col min="3" max="3" width="17"/>
     <col min="4" max="4" width="13" style="2"/>
     <col min="5" max="5" width="19"/>
-    <col min="6" max="6" width="8.7109375"/>
-    <col min="7" max="7" width="15.5703125"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="6" max="6" width="8.6640625"/>
+    <col min="7" max="7" width="15.5546875"/>
+    <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -825,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -845,7 +845,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -868,7 +868,7 @@
         <v>43392</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -926,7 +926,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -949,7 +949,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -967,7 +967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>43379</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="H32" t="s">
         <v>70</v>
@@ -1480,22 +1480,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>6</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="6" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="6" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>9</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>10</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>11</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>13</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>14</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>15</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>17</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>18</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>19</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>43407</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>21</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>24</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>25</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>26</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>27</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>28</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>29</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>30</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>31</v>
       </c>
@@ -2095,32 +2095,56 @@
         <v>43416</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>32</v>
+      </c>
       <c r="B25" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="23">
+        <v>33</v>
+      </c>
       <c r="B26" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>34</v>
+      </c>
       <c r="B27" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="23">
+        <v>35</v>
+      </c>
       <c r="B28" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>36</v>
+      </c>
       <c r="B29" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="23">
+        <v>37</v>
+      </c>
       <c r="B30" s="11" t="s">
         <v>86</v>
       </c>

</xml_diff>